<commit_message>
add table read_messages, mark messages as read, fix import excel
</commit_message>
<xml_diff>
--- a/public/templates/excel/import_users_ja.xlsx
+++ b/public/templates/excel/import_users_ja.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
+    <sheet name="Departments" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Member</t>
   </si>
@@ -47,6 +48,42 @@
   </si>
   <si>
     <t>No.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">住宅事業部チーム </t>
+  </si>
+  <si>
+    <t>FREEDOMのチーム</t>
+  </si>
+  <si>
+    <t>経理チーム経理チーム</t>
+  </si>
+  <si>
+    <t>解析チーム</t>
+  </si>
+  <si>
+    <t>業務チーム</t>
+  </si>
+  <si>
+    <t>オートキャドチーム</t>
+  </si>
+  <si>
+    <t xml:space="preserve">住宅事業部チーム Level 2.1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">住宅事業部チーム Level 2.1.1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">住宅事業部チーム Level 2.1.2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">住宅事業部チーム Level 2.1.3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">住宅事業部チーム Level 2.2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">住宅事業部チーム Level 2.3 </t>
   </si>
 </sst>
 </file>
@@ -159,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -208,6 +245,42 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -515,7 +588,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -528,7 +601,7 @@
     <col min="6" max="6" width="19" style="10" customWidth="1"/>
     <col min="7" max="7" width="44.28515625" style="10" customWidth="1"/>
     <col min="8" max="8" width="23.28515625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="31" style="5" customWidth="1"/>
+    <col min="9" max="9" width="31" style="26" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" style="5" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
@@ -558,7 +631,7 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -576,7 +649,9 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="I2" s="27" t="s">
+        <v>11</v>
+      </c>
       <c r="J2" s="11" t="s">
         <v>0</v>
       </c>
@@ -592,7 +667,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="I3" s="28"/>
       <c r="J3" s="6" t="s">
         <v>0</v>
       </c>
@@ -608,7 +683,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="I4" s="24"/>
       <c r="J4" s="6" t="s">
         <v>0</v>
       </c>
@@ -624,7 +699,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="I5" s="24"/>
       <c r="J5" s="6" t="s">
         <v>0</v>
       </c>
@@ -640,7 +715,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="I6" s="25"/>
       <c r="J6" s="8" t="s">
         <v>0</v>
       </c>
@@ -653,5 +728,139 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Departments!$B$2:$B$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="22">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="22">
+        <v>4</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="22">
+        <v>5</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="22">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
+        <v>8</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="22">
+        <v>9</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="22">
+        <v>10</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="22">
+        <v>11</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="23">
+        <v>12</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>